<commit_message>
Update testing and CN.
</commit_message>
<xml_diff>
--- a/2_design/asim/artifacts/testing/analyze-item.xlsx
+++ b/2_design/asim/artifacts/testing/analyze-item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GoogleDrive\todo\working\projects\sim\2_design\asim\artifacts\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D02F9AA-6E09-4040-9ABF-129660E9465A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204A1879-11BD-4B45-A065-66D4007FF5FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{8DB95D20-6883-4AA3-B7D2-5A0EAC39C354}"/>
   </bookViews>
@@ -881,13 +881,13 @@
                   <c:v>3.3538049570698454E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2070109551855352E-2</c:v>
+                  <c:v>1.7647872016693471E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>3.3843793470341894E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2364134233328546E-2</c:v>
+                  <c:v>1.8036730401939958E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>3.3535323828952593E-2</c:v>
@@ -8542,7 +8542,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9096,15 +9096,19 @@
       <c r="D16" s="1">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2.9600000000000001E-2</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1">
         <f t="shared" si="0"/>
-        <v>1.2233333333333332E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -9156,15 +9160,19 @@
       <c r="D18" s="1">
         <v>1.83E-2</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3.0200000000000001E-2</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1">
         <f t="shared" si="0"/>
-        <v>1.2533333333333334E-2</v>
+        <v>1.84E-2</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -9718,7 +9726,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10272,15 +10280,19 @@
       <c r="D16" s="1">
         <v>0.90239999999999998</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="E16" s="1">
+        <v>0.90049999999999997</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.8962</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1">
         <f t="shared" si="0"/>
-        <v>0.9046333333333334</v>
+        <v>0.90212000000000003</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -10332,15 +10344,19 @@
       <c r="D18" s="1">
         <v>0.91369999999999996</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1">
+        <v>0.91159999999999997</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.90869999999999995</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1">
         <f t="shared" si="0"/>
-        <v>0.91586666666666672</v>
+        <v>0.91357999999999995</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -11154,15 +11170,15 @@
       </c>
       <c r="B16" s="1">
         <f>Precision!K16</f>
-        <v>1.2233333333333332E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="C16" s="1">
         <f>Recall!K16</f>
-        <v>0.9046333333333334</v>
+        <v>0.90212000000000003</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>1.2070109551855352E-2</v>
+        <v>1.7647872016693471E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -11188,15 +11204,15 @@
       </c>
       <c r="B18" s="1">
         <f>Precision!K18</f>
-        <v>1.2533333333333334E-2</v>
+        <v>1.84E-2</v>
       </c>
       <c r="C18" s="1">
         <f>Recall!K18</f>
-        <v>0.91586666666666672</v>
+        <v>0.91357999999999995</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>1.2364134233328546E-2</v>
+        <v>1.8036730401939958E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>